<commit_message>
Created Function for Gaussian Quadrature Scheme, and exported it to the Averaged Intensities files.
</commit_message>
<xml_diff>
--- a/JupyterNotebooks/AveragedIntensites/AlphaFiberF-HW10.xlsx
+++ b/JupyterNotebooks/AveragedIntensites/AlphaFiberF-HW10.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="AlphaFiberF-HW10.xpc" sheetId="1" r:id="rId1"/>
+    <sheet name="AlphaFiberF" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>HKL</t>
   </si>
@@ -446,7 +446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -949,7 +949,7 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>0.9818658657972131</v>
+        <v>0.9818658657972137</v>
       </c>
       <c r="D13">
         <v>0.9973954634041032</v>
@@ -958,7 +958,7 @@
         <v>0.9968082978711924</v>
       </c>
       <c r="F13">
-        <v>0.9818658657972131</v>
+        <v>0.9818658657972137</v>
       </c>
       <c r="G13">
         <v>0.9918081981030068</v>
@@ -976,10 +976,10 @@
         <v>0.9971018806376478</v>
       </c>
       <c r="L13">
-        <v>0.9894838732174305</v>
+        <v>0.9894838732174307</v>
       </c>
       <c r="M13">
-        <v>0.9926044986113151</v>
+        <v>0.9926044986113153</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1062,6 +1062,47 @@
       </c>
       <c r="M15">
         <v>0.9855094574666232</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>1.732273679167148</v>
+      </c>
+      <c r="D16">
+        <v>1.686442167232839</v>
+      </c>
+      <c r="E16">
+        <v>0.7414874669677609</v>
+      </c>
+      <c r="F16">
+        <v>1.732273679167148</v>
+      </c>
+      <c r="G16">
+        <v>0.9880047329540944</v>
+      </c>
+      <c r="H16">
+        <v>1.071215803390088</v>
+      </c>
+      <c r="I16">
+        <v>0.8604059345742562</v>
+      </c>
+      <c r="J16">
+        <v>1.686442167232839</v>
+      </c>
+      <c r="K16">
+        <v>1.2139648171003</v>
+      </c>
+      <c r="L16">
+        <v>1.473119248133724</v>
+      </c>
+      <c r="M16">
+        <v>1.179971630714365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Cross-Platform functionality with jupyter notebooks. Ran Averaged Intensities code to fix Gaussian Quadrature naming.
</commit_message>
<xml_diff>
--- a/JupyterNotebooks/AveragedIntensites/AlphaFiberF-HW10.xlsx
+++ b/JupyterNotebooks/AveragedIntensites/AlphaFiberF-HW10.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>HKL</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>HexGrid-60degTilt5degRes</t>
+  </si>
+  <si>
+    <t>Gaussian-Quadrature</t>
   </si>
   <si>
     <t>[1, 1, 0]</t>
@@ -498,37 +501,37 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1069,7 +1072,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>1.732273679167148</v>

</xml_diff>

<commit_message>
Fixed line numbers for plotting
See issue #3
</commit_message>
<xml_diff>
--- a/JupyterNotebooks/AveragedIntensites/AlphaFiberF-HW10.xlsx
+++ b/JupyterNotebooks/AveragedIntensites/AlphaFiberF-HW10.xlsx
@@ -952,7 +952,7 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>0.9818658657972137</v>
+        <v>0.9818658657972131</v>
       </c>
       <c r="D13">
         <v>0.9973954634041032</v>
@@ -961,7 +961,7 @@
         <v>0.9968082978711924</v>
       </c>
       <c r="F13">
-        <v>0.9818658657972137</v>
+        <v>0.9818658657972131</v>
       </c>
       <c r="G13">
         <v>0.9918081981030068</v>
@@ -979,10 +979,10 @@
         <v>0.9971018806376478</v>
       </c>
       <c r="L13">
-        <v>0.9894838732174307</v>
+        <v>0.9894838732174305</v>
       </c>
       <c r="M13">
-        <v>0.9926044986113153</v>
+        <v>0.9926044986113151</v>
       </c>
     </row>
     <row r="14" spans="1:13">

</xml_diff>

<commit_message>
Ran code for averaged intensities on spiral schemes
</commit_message>
<xml_diff>
--- a/JupyterNotebooks/AveragedIntensites/AlphaFiberF-HW10.xlsx
+++ b/JupyterNotebooks/AveragedIntensites/AlphaFiberF-HW10.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>HKL</t>
   </si>
@@ -40,6 +40,18 @@
     <t>Ring Perpendicular to TD</t>
   </si>
   <si>
+    <t>Gaussian-Quadrature</t>
+  </si>
+  <si>
+    <t>Spiral-90deg-10rot-5space</t>
+  </si>
+  <si>
+    <t>Spiral-90deg-15rot-5space</t>
+  </si>
+  <si>
+    <t>Spiral-90deg-10rot-3space</t>
+  </si>
+  <si>
     <t>NoRotation-tilt60deg</t>
   </si>
   <si>
@@ -56,9 +68,6 @@
   </si>
   <si>
     <t>HexGrid-60degTilt5degRes</t>
-  </si>
-  <si>
-    <t>Gaussian-Quadrature</t>
   </si>
   <si>
     <t>[1, 1, 0]</t>
@@ -449,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -501,37 +510,37 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -829,37 +838,37 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>0.3046320000000002</v>
+        <v>1.732273679167148</v>
       </c>
       <c r="D10">
-        <v>2.737640000000001</v>
+        <v>1.686442167232839</v>
       </c>
       <c r="E10">
-        <v>1.306147999999999</v>
+        <v>0.7414874669677609</v>
       </c>
       <c r="F10">
-        <v>0.3046320000000002</v>
+        <v>1.732273679167148</v>
       </c>
       <c r="G10">
-        <v>0.8309159999999988</v>
+        <v>0.9880047329540944</v>
       </c>
       <c r="H10">
-        <v>2.474299999999999</v>
+        <v>1.071215803390088</v>
       </c>
       <c r="I10">
-        <v>0.8105199999999971</v>
+        <v>0.8604059345742562</v>
       </c>
       <c r="J10">
-        <v>2.737640000000001</v>
+        <v>1.686442167232839</v>
       </c>
       <c r="K10">
-        <v>2.021894</v>
+        <v>1.2139648171003</v>
       </c>
       <c r="L10">
-        <v>1.163263</v>
+        <v>1.473119248133724</v>
       </c>
       <c r="M10">
-        <v>1.410692666666666</v>
+        <v>1.179971630714365</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -870,37 +879,37 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>0.8775160230008457</v>
       </c>
       <c r="D11">
-        <v>3.027662500000005</v>
+        <v>1.647741017954402</v>
       </c>
       <c r="E11">
-        <v>1.473899999999997</v>
+        <v>1.140059471635869</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>0.8775160230008457</v>
       </c>
       <c r="G11">
-        <v>0.843062500000001</v>
+        <v>0.5938586813806822</v>
       </c>
       <c r="H11">
-        <v>2.765837500000004</v>
+        <v>2.583175435397902</v>
       </c>
       <c r="I11">
-        <v>0.8463874999999991</v>
+        <v>0.868989607860985</v>
       </c>
       <c r="J11">
-        <v>3.027662500000005</v>
+        <v>1.647741017954402</v>
       </c>
       <c r="K11">
-        <v>2.250781250000001</v>
+        <v>1.393900244795136</v>
       </c>
       <c r="L11">
-        <v>1.125390625000001</v>
+        <v>1.135708133897991</v>
       </c>
       <c r="M11">
-        <v>1.492808333333334</v>
+        <v>1.285223372871781</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -911,37 +920,37 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>0.4133131813888014</v>
+        <v>0.8756978369841125</v>
       </c>
       <c r="D12">
-        <v>2.140809199616004</v>
+        <v>1.651696757827705</v>
       </c>
       <c r="E12">
-        <v>1.257639591935999</v>
+        <v>1.139644025183083</v>
       </c>
       <c r="F12">
-        <v>0.4133131813888014</v>
+        <v>0.8756978369841125</v>
       </c>
       <c r="G12">
-        <v>0.9186980947967979</v>
+        <v>0.5955545344539952</v>
       </c>
       <c r="H12">
-        <v>1.981674290073604</v>
+        <v>2.578670456575261</v>
       </c>
       <c r="I12">
-        <v>0.9048020599808049</v>
+        <v>0.8681268382183878</v>
       </c>
       <c r="J12">
-        <v>2.140809199616004</v>
+        <v>1.651696757827705</v>
       </c>
       <c r="K12">
-        <v>1.699224395776001</v>
+        <v>1.395670391505394</v>
       </c>
       <c r="L12">
-        <v>1.056268788582401</v>
+        <v>1.135684114244753</v>
       </c>
       <c r="M12">
-        <v>1.269489402965335</v>
+        <v>1.284898408207091</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -952,37 +961,37 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>0.9818658657972131</v>
+        <v>0.8768895849716551</v>
       </c>
       <c r="D13">
-        <v>0.9973954634041032</v>
+        <v>1.648122290621395</v>
       </c>
       <c r="E13">
-        <v>0.9968082978711924</v>
+        <v>1.140056396954657</v>
       </c>
       <c r="F13">
-        <v>0.9818658657972131</v>
+        <v>0.8768895849716551</v>
       </c>
       <c r="G13">
-        <v>0.9918081981030068</v>
+        <v>0.5943733154820969</v>
       </c>
       <c r="H13">
-        <v>0.9947990907591019</v>
+        <v>2.581797812965256</v>
       </c>
       <c r="I13">
-        <v>0.9929500757332735</v>
+        <v>0.868462399832437</v>
       </c>
       <c r="J13">
-        <v>0.9973954634041032</v>
+        <v>1.648122290621395</v>
       </c>
       <c r="K13">
-        <v>0.9971018806376478</v>
+        <v>1.394089343788026</v>
       </c>
       <c r="L13">
-        <v>0.9894838732174305</v>
+        <v>1.135489464379841</v>
       </c>
       <c r="M13">
-        <v>0.9926044986113151</v>
+        <v>1.284950300137916</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -993,37 +1002,37 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>1.190184492971753</v>
+        <v>0.3046320000000002</v>
       </c>
       <c r="D14">
-        <v>0.9466316812117093</v>
+        <v>2.737640000000001</v>
       </c>
       <c r="E14">
-        <v>0.9965097633198127</v>
+        <v>1.306147999999999</v>
       </c>
       <c r="F14">
-        <v>1.190184492971753</v>
+        <v>0.3046320000000002</v>
       </c>
       <c r="G14">
-        <v>0.9683137724766275</v>
+        <v>0.8309159999999988</v>
       </c>
       <c r="H14">
-        <v>1.030006979687314</v>
+        <v>2.474299999999999</v>
       </c>
       <c r="I14">
-        <v>0.9375822955243313</v>
+        <v>0.8105199999999971</v>
       </c>
       <c r="J14">
-        <v>0.9466316812117093</v>
+        <v>2.737640000000001</v>
       </c>
       <c r="K14">
-        <v>0.971570722265761</v>
+        <v>2.021894</v>
       </c>
       <c r="L14">
-        <v>1.080877607618757</v>
+        <v>1.163263</v>
       </c>
       <c r="M14">
-        <v>1.011538164198591</v>
+        <v>1.410692666666666</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1034,37 +1043,37 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>1.023928482688378</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>0.9518127726826778</v>
+        <v>3.027662500000005</v>
       </c>
       <c r="E15">
-        <v>0.9877579946533892</v>
+        <v>1.473899999999997</v>
       </c>
       <c r="F15">
-        <v>1.023928482688378</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>0.9703618010410472</v>
+        <v>0.843062500000001</v>
       </c>
       <c r="H15">
-        <v>0.9818261672495591</v>
+        <v>2.765837500000004</v>
       </c>
       <c r="I15">
-        <v>0.997369526484688</v>
+        <v>0.8463874999999991</v>
       </c>
       <c r="J15">
-        <v>0.9518127726826778</v>
+        <v>3.027662500000005</v>
       </c>
       <c r="K15">
-        <v>0.9697853836680335</v>
+        <v>2.250781250000001</v>
       </c>
       <c r="L15">
-        <v>0.9968569331782057</v>
+        <v>1.125390625000001</v>
       </c>
       <c r="M15">
-        <v>0.9855094574666232</v>
+        <v>1.492808333333334</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1075,37 +1084,160 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>1.732273679167148</v>
+        <v>0.4133131813888014</v>
       </c>
       <c r="D16">
-        <v>1.686442167232839</v>
+        <v>2.140809199616004</v>
       </c>
       <c r="E16">
-        <v>0.7414874669677609</v>
+        <v>1.257639591935999</v>
       </c>
       <c r="F16">
-        <v>1.732273679167148</v>
+        <v>0.4133131813888014</v>
       </c>
       <c r="G16">
-        <v>0.9880047329540944</v>
+        <v>0.9186980947967979</v>
       </c>
       <c r="H16">
-        <v>1.071215803390088</v>
+        <v>1.981674290073604</v>
       </c>
       <c r="I16">
-        <v>0.8604059345742562</v>
+        <v>0.9048020599808049</v>
       </c>
       <c r="J16">
-        <v>1.686442167232839</v>
+        <v>2.140809199616004</v>
       </c>
       <c r="K16">
-        <v>1.2139648171003</v>
+        <v>1.699224395776001</v>
       </c>
       <c r="L16">
-        <v>1.473119248133724</v>
+        <v>1.056268788582401</v>
       </c>
       <c r="M16">
-        <v>1.179971630714365</v>
+        <v>1.269489402965335</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>0.9818658657972137</v>
+      </c>
+      <c r="D17">
+        <v>0.9973954634041032</v>
+      </c>
+      <c r="E17">
+        <v>0.9968082978711924</v>
+      </c>
+      <c r="F17">
+        <v>0.9818658657972137</v>
+      </c>
+      <c r="G17">
+        <v>0.9918081981030068</v>
+      </c>
+      <c r="H17">
+        <v>0.9947990907591019</v>
+      </c>
+      <c r="I17">
+        <v>0.9929500757332735</v>
+      </c>
+      <c r="J17">
+        <v>0.9973954634041032</v>
+      </c>
+      <c r="K17">
+        <v>0.9971018806376478</v>
+      </c>
+      <c r="L17">
+        <v>0.9894838732174307</v>
+      </c>
+      <c r="M17">
+        <v>0.9926044986113153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>1.190184492971753</v>
+      </c>
+      <c r="D18">
+        <v>0.9466316812117093</v>
+      </c>
+      <c r="E18">
+        <v>0.9965097633198127</v>
+      </c>
+      <c r="F18">
+        <v>1.190184492971753</v>
+      </c>
+      <c r="G18">
+        <v>0.9683137724766275</v>
+      </c>
+      <c r="H18">
+        <v>1.030006979687314</v>
+      </c>
+      <c r="I18">
+        <v>0.9375822955243313</v>
+      </c>
+      <c r="J18">
+        <v>0.9466316812117093</v>
+      </c>
+      <c r="K18">
+        <v>0.971570722265761</v>
+      </c>
+      <c r="L18">
+        <v>1.080877607618757</v>
+      </c>
+      <c r="M18">
+        <v>1.011538164198591</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>1.023928482688378</v>
+      </c>
+      <c r="D19">
+        <v>0.9518127726826778</v>
+      </c>
+      <c r="E19">
+        <v>0.9877579946533892</v>
+      </c>
+      <c r="F19">
+        <v>1.023928482688378</v>
+      </c>
+      <c r="G19">
+        <v>0.9703618010410472</v>
+      </c>
+      <c r="H19">
+        <v>0.9818261672495591</v>
+      </c>
+      <c r="I19">
+        <v>0.997369526484688</v>
+      </c>
+      <c r="J19">
+        <v>0.9518127726826778</v>
+      </c>
+      <c r="K19">
+        <v>0.9697853836680335</v>
+      </c>
+      <c r="L19">
+        <v>0.9968569331782057</v>
+      </c>
+      <c r="M19">
+        <v>0.9855094574666232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>